<commit_message>
FT MT POS KPI template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2020/POS_VALIDATION/OUTPUT/PoS 2020 - FT.xlsx
+++ b/Projects/CCRU/Data/KPIs_2020/POS_VALIDATION/OUTPUT/PoS 2020 - FT.xlsx
@@ -1250,7 +1250,7 @@
     <t xml:space="preserve">Coca-Cola</t>
   </si>
   <si>
-    <t xml:space="preserve">SSD 1 door; SSD 1.5 door; Mixed 1 door; Mixed  1.5 door; SS_SSD 1 door; SS_SSD 1.5 door; SS_Mixed 1 door; SS_Mixed  1.5 door</t>
+    <t xml:space="preserve">SSD 1 door; SSD 1.5 door; Mixed 1 door; Mixed  1.5 door; SS_SSD 1 door; SS_SSD 1.5 door; SS_Mixed 1 door; SS_Mixed  1.5 door; CA_SSD 1 door; CA_SSD 1.5 door; CA_Mixed 1 door; CA_Mixed  1.5 door</t>
   </si>
   <si>
     <t xml:space="preserve">80
@@ -1275,7 +1275,7 @@
     <t xml:space="preserve">2, 3</t>
   </si>
   <si>
-    <t xml:space="preserve">SSD 1 door; NCB 1 door; Mixed 1 door; SSD 1.5 door; NSB  1.5 door; Mixed  1.5 door; SSDFL 1 door; SSDFL 1.5 door; SS_SSD 1 door; SS_NCB 1 door; SS_Mixed 1 door; SS_SSD 1.5 door; SS_NSB  1.5 door; SS_Mixed  1.5 door; SS_SSDFL 1 door; SS_SSDFL 1.5 door</t>
+    <t xml:space="preserve">SSD 1 door; NCB 1 door; Mixed 1 door; SSD 1.5 door; NSB  1.5 door; Mixed  1.5 door; SSDFL 1 door; SSDFL 1.5 door; SS_SSD 1 door; SS_NCB 1 door; SS_Mixed 1 door; SS_SSD 1.5 door; SS_NSB  1.5 door; SS_Mixed  1.5 door; SS_SSDFL 1 door; SS_SSDFL 1.5 door; CA_SSD 1 door; CA_NCB 1 door; CA_Mixed 1 door; CA_SSD 1.5 door; CA_NSB  1.5 door; CA_Mixed  1.5 door; CA_SSDFL 1 door; CA_SSDFL 1.5 door</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler: Merch Priorty STD coca- cola shelf 2-3</t>

</xml_diff>